<commit_message>
updated code with 3 data sessions
ran 3 data sessions and created table
</commit_message>
<xml_diff>
--- a/ExcelFiles/s3_good_trials_GraspObject.xlsx
+++ b/ExcelFiles/s3_good_trials_GraspObject.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macthurston\Documents\GitHub\project_grasp_object_interaction\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65CAA00-7D9F-4696-B918-AA7D72F71103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7166F73-8FB3-467E-BBF3-7908FB98E654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-4470" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -91,8 +90,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,7 +375,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,22 +398,22 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -496,9 +495,30 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="2">
+        <v>20230803</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>